<commit_message>
More Petit evolutions' brainstorming
</commit_message>
<xml_diff>
--- a/Custom Cards/Custom Card Types/Evolution Monsters/Petit Evolutions/Petit Evolutions.xlsx
+++ b/Custom Cards/Custom Card Types/Evolution Monsters/Petit Evolutions/Petit Evolutions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Custom Cards\Custom Card Types\Evolution Monsters\Petit Evolutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2EC46D-93B4-4E2F-8DFE-88D49E00BE45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB9DF0D-6486-4BE5-92BD-EC733B8F9A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>WATER</t>
   </si>
   <si>
-    <t>Alexandrite Dragon / Krystal Dragon</t>
-  </si>
-  <si>
     <t>Thunder</t>
   </si>
   <si>
@@ -159,15 +156,6 @@
     <t>Baby Dragon</t>
   </si>
   <si>
-    <t>Snow, Dragon of the Blizzard</t>
-  </si>
-  <si>
-    <t>Ice, Dragon of the Glacier</t>
-  </si>
-  <si>
-    <t>Polar, Guardian Dragon of Auroras</t>
-  </si>
-  <si>
     <t>Polar</t>
   </si>
   <si>
@@ -235,6 +223,18 @@
   </si>
   <si>
     <t>Angel of Marriage</t>
+  </si>
+  <si>
+    <t>Aurora, Guardian of the Radiant Skies</t>
+  </si>
+  <si>
+    <t>Glacier, Incarnation of the Frozen Tempest</t>
+  </si>
+  <si>
+    <t>White Night Dragon / Alexandrite Dragon / Krystal Dragon</t>
+  </si>
+  <si>
+    <t>Snow, Wyvern of the Blizzard</t>
   </si>
 </sst>
 </file>
@@ -664,7 +664,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,10 +678,10 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -701,10 +701,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>5</v>
@@ -715,12 +715,12 @@
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>3</v>
@@ -729,7 +729,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>9</v>
@@ -739,13 +739,13 @@
       <c r="A5" s="2"/>
       <c r="B5"/>
       <c r="C5" s="7" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -770,54 +770,54 @@
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>13</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -826,83 +826,83 @@
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>21</v>
-      </c>
       <c r="C12" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="C13" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="E14" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15"/>
       <c r="C15" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D15" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -910,65 +910,65 @@
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19"/>
       <c r="C19" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C21" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>